<commit_message>
change trial treatment identity
</commit_message>
<xml_diff>
--- a/exploratory/data/tables/#keto-rev_treatmentinitiation_data.xlsx
+++ b/exploratory/data/tables/#keto-rev_treatmentinitiation_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahbukovac/Desktop/#keto-rev/modified xlsx tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2637CE51-473A-A74F-9F84-BD2ABE2227B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E3F94-3B41-7747-A70E-CB248D04382C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2680" windowWidth="25080" windowHeight="17340" xr2:uid="{8F4EEB4E-841A-FB4C-9F52-3861DEB61C98}"/>
   </bookViews>
@@ -606,7 +606,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>2007</v>

</xml_diff>

<commit_message>
reorganize and update repo
</commit_message>
<xml_diff>
--- a/exploratory/data/tables/#keto-rev_treatmentinitiation_data.xlsx
+++ b/exploratory/data/tables/#keto-rev_treatmentinitiation_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahbukovac/Desktop/#keto-rev/modified xlsx tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E3F94-3B41-7747-A70E-CB248D04382C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62304236-FDC9-5143-959A-2CE3DD8FDE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2680" windowWidth="25080" windowHeight="17340" xr2:uid="{8F4EEB4E-841A-FB4C-9F52-3861DEB61C98}"/>
+    <workbookView xWindow="6420" yWindow="2780" windowWidth="25080" windowHeight="17340" xr2:uid="{8F4EEB4E-841A-FB4C-9F52-3861DEB61C98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>Targeted Disruption to Cancer Metabolism Through Dietary Macronutrient Modification</t>
   </si>
@@ -192,12 +192,21 @@
   <si>
     <t>Initiation</t>
   </si>
+  <si>
+    <t>MB Endpoint</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +250,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,13 +277,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,12 +622,12 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -624,8 +640,11 @@
       <c r="D1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -638,8 +657,11 @@
       <c r="D2">
         <v>2015</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -652,8 +674,11 @@
       <c r="D3">
         <v>2017</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -666,8 +691,11 @@
       <c r="D4">
         <v>2017</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -680,8 +708,11 @@
       <c r="D5">
         <v>2012</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -694,8 +725,11 @@
       <c r="D6">
         <v>2017</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -708,8 +742,11 @@
       <c r="D7">
         <v>2017</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -722,8 +759,11 @@
       <c r="D8">
         <v>2007</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -736,8 +776,11 @@
       <c r="D9">
         <v>2006</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -750,8 +793,11 @@
       <c r="D10">
         <v>2013</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -764,8 +810,11 @@
       <c r="D11">
         <v>2015</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -778,8 +827,11 @@
       <c r="D12">
         <v>2007</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -792,8 +844,11 @@
       <c r="D13">
         <v>2015</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -806,8 +861,11 @@
       <c r="D14">
         <v>2015</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -820,8 +878,11 @@
       <c r="D15">
         <v>2020</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -834,8 +895,11 @@
       <c r="D16">
         <v>2020</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -848,6 +912,10 @@
       <c r="D17">
         <v>2014</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -862,6 +930,9 @@
       <c r="D18">
         <v>2017</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -876,6 +947,9 @@
       <c r="D19">
         <v>2014</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -890,6 +964,9 @@
       <c r="D20">
         <v>2010</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -903,6 +980,9 @@
       </c>
       <c r="D21">
         <v>2016</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>